<commit_message>
I will not sleep until these data are good!
</commit_message>
<xml_diff>
--- a/data/23 nrec decomp biomass.xlsx
+++ b/data/23 nrec decomp biomass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/2023_nrec_decomp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6978E4-A792-A347-9855-C8C91DACDF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FF7D40-478F-7D44-8168-2DFA0E185D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{4A753238-9247-8848-863F-14539E74CA07}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="30">
   <si>
     <t>crop</t>
   </si>
@@ -485,8 +485,8 @@
   <dimension ref="A1:K401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A346" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N363" sqref="N363"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J300" sqref="J300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10192,10 +10192,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G282">
-        <v>22.3</v>
+        <v>23.9</v>
       </c>
       <c r="H282">
         <v>0.1</v>
+      </c>
+      <c r="I282" t="s">
+        <v>13</v>
+      </c>
+      <c r="J282">
+        <v>23.9</v>
+      </c>
+      <c r="K282">
+        <v>1.7290000000000001</v>
       </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.2">
@@ -10532,7 +10541,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G293">
-        <v>4.5</v>
+        <v>10.6</v>
       </c>
       <c r="H293">
         <v>0.1</v>
@@ -10709,16 +10718,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G299">
-        <v>6.1</v>
+        <v>11.17</v>
       </c>
       <c r="H299">
         <v>0.1</v>
       </c>
+      <c r="I299" t="s">
+        <v>13</v>
+      </c>
       <c r="J299">
-        <v>5.3280000000000003</v>
+        <v>11.17</v>
       </c>
       <c r="K299">
-        <v>1.6319999999999999</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>